<commit_message>
Excel Parite 3 fini, il manque l'interpretation
</commit_message>
<xml_diff>
--- a/EvaluationDesPerformances.xlsx
+++ b/EvaluationDesPerformances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxencenaud/Desktop/Programmation/2A/ES201/ES201_TD4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB61D75C-2483-6F41-8D39-334DEA74109C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E073F2B-005B-144E-B602-08266E4ED67B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{E820CF42-18EB-2C49-9FDD-82D7986B5BCD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
   <si>
     <t>Cache Size</t>
   </si>
@@ -86,40 +86,10 @@
     <t>bpred_bimod.bpred_dir_rate</t>
   </si>
   <si>
-    <t>0.0009</t>
-  </si>
-  <si>
     <t>Exercice 5</t>
   </si>
   <si>
     <t>32dB</t>
-  </si>
-  <si>
-    <t>0.8035</t>
-  </si>
-  <si>
-    <t>1.2445</t>
-  </si>
-  <si>
-    <t>0.8324</t>
-  </si>
-  <si>
-    <t>0.0149</t>
-  </si>
-  <si>
-    <t>0.0424</t>
-  </si>
-  <si>
-    <t>0.0106</t>
-  </si>
-  <si>
-    <t>0.0193</t>
-  </si>
-  <si>
-    <t>0.0016</t>
-  </si>
-  <si>
-    <t>0.8256</t>
   </si>
 </sst>
 </file>
@@ -1905,11 +1875,8 @@
               <a:rPr lang="fr-FR" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Cortex A15 - Hiérarchie Mémoire - Dijkstra</a:t>
+              <a:t>Cortex A15 - Hiérarchie Mémoire - BlowFish</a:t>
             </a:r>
-            <a:endParaRPr lang="fr-FR" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2321,6 +2288,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cortex A15 - IPC - BLowFish</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2551,6 +2543,854 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="605594080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Cortex A15 - Hiérarchie Mémoire - Dijkstra</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$G$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>il1_miss_rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$B$33:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2dB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4dB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8dB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16dB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32dB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$G$33:$G$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.49E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.06E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-95BF-6347-BA6A-D52A27F6C449}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$H$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dl1_miss_rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$B$33:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2dB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4dB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8dB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16dB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32dB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$H$33:$H$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.24E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-95BF-6347-BA6A-D52A27F6C449}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$I$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ul2_miss_rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$B$33:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2dB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4dB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8dB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16dB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32dB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$I$33:$I$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.9999999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0999999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0899999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-95BF-6347-BA6A-D52A27F6C449}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="643249488"/>
+        <c:axId val="645144368"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="643249488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="645144368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="645144368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="643249488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cortex</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> A15 - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>IPC - BlowFish</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$F$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IPC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$B$33:$B$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2dB</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4dB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8dB</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16dB</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32dB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$F$33:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.80349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85529999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87060000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88300000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE39-D44E-A126-6D238FFF5745}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="595098416"/>
+        <c:axId val="640609968"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="595098416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="640609968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="640609968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595098416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2846,6 +3686,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5362,6 +6282,1012 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6084,6 +8010,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Graphique 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A05F8FFB-A637-0143-B062-35ECCFDA3ED5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Graphique 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3D3EEE1-C9DF-304A-991A-EE2A05DF4154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6386,8 +8384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3749EF-EF44-254D-B120-5281889EAB56}">
   <dimension ref="A2:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6760,7 +8758,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -6913,7 +8911,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29">
         <v>7677</v>
@@ -6982,23 +8980,23 @@
       <c r="D33">
         <v>68301832</v>
       </c>
-      <c r="E33" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H33" t="s">
-        <v>24</v>
-      </c>
-      <c r="I33" t="s">
-        <v>17</v>
-      </c>
-      <c r="J33" t="s">
-        <v>22</v>
+      <c r="E33">
+        <v>1.2444999999999999</v>
+      </c>
+      <c r="F33">
+        <v>0.80349999999999999</v>
+      </c>
+      <c r="G33">
+        <v>1.49E-2</v>
+      </c>
+      <c r="H33">
+        <v>4.24E-2</v>
+      </c>
+      <c r="I33">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J33">
+        <v>0.83240000000000003</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
@@ -7008,17 +9006,26 @@
       <c r="C34">
         <v>54881612</v>
       </c>
-      <c r="G34" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" t="s">
-        <v>27</v>
-      </c>
-      <c r="J34" t="s">
-        <v>28</v>
+      <c r="D34">
+        <v>66566219</v>
+      </c>
+      <c r="E34">
+        <v>1.2129000000000001</v>
+      </c>
+      <c r="F34">
+        <v>0.82450000000000001</v>
+      </c>
+      <c r="G34">
+        <v>1.06E-2</v>
+      </c>
+      <c r="H34">
+        <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="I34">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="J34">
+        <v>0.8256</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
@@ -7028,6 +9035,27 @@
       <c r="C35">
         <v>54881612</v>
       </c>
+      <c r="D35">
+        <v>64165602</v>
+      </c>
+      <c r="E35">
+        <v>1.1692</v>
+      </c>
+      <c r="F35">
+        <v>0.85529999999999995</v>
+      </c>
+      <c r="G35">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="H35">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="I35">
+        <v>3.8E-3</v>
+      </c>
+      <c r="J35">
+        <v>0.82</v>
+      </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
@@ -7036,13 +9064,55 @@
       <c r="C36">
         <v>54881612</v>
       </c>
+      <c r="D36">
+        <v>63039810</v>
+      </c>
+      <c r="E36">
+        <v>1.1487000000000001</v>
+      </c>
+      <c r="F36">
+        <v>0.87060000000000004</v>
+      </c>
+      <c r="G36">
+        <v>1.9E-3</v>
+      </c>
+      <c r="H36">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="I36">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="J36">
+        <v>0.81799999999999995</v>
+      </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37">
         <v>54881612</v>
+      </c>
+      <c r="D37">
+        <v>62155178</v>
+      </c>
+      <c r="E37">
+        <v>1.1325000000000001</v>
+      </c>
+      <c r="F37">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="I37">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="J37">
+        <v>0.81740000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>